<commit_message>
fix minor login bug
</commit_message>
<xml_diff>
--- a/public/database/csmc-database.xlsx
+++ b/public/database/csmc-database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Supahotfile\pkw\csmc\public\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E7E46B-6C5B-46A3-A35A-CF0B92438BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83374E68-FC54-4B3F-B8AA-A7035CD1C662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6202" uniqueCount="2075">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6203" uniqueCount="2076">
   <si>
     <t>ประทับเวลา</t>
   </si>
@@ -6246,6 +6246,9 @@
   </si>
   <si>
     <t>1839902267328</t>
+  </si>
+  <si>
+    <t>1839902244697</t>
   </si>
 </sst>
 </file>
@@ -22134,7 +22137,7 @@
   <dimension ref="A1:V356"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="22.2" x14ac:dyDescent="0.6"/>
@@ -22777,8 +22780,8 @@
       <c r="I10" s="19">
         <v>12</v>
       </c>
-      <c r="J10" s="20">
-        <v>1839902244697</v>
+      <c r="J10" s="20" t="s">
+        <v>2075</v>
       </c>
       <c r="K10" s="19">
         <v>842436098</v>

</xml_diff>

<commit_message>
update mean & total score
</commit_message>
<xml_diff>
--- a/public/database/csmc-database.xlsx
+++ b/public/database/csmc-database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Supahotfile\pkw\csmc\public\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83374E68-FC54-4B3F-B8AA-A7035CD1C662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D930424B-FF04-4E95-8CCC-BFB4EC84D740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6203" uniqueCount="2076">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6202" uniqueCount="2075">
   <si>
     <t>ประทับเวลา</t>
   </si>
@@ -6240,9 +6240,6 @@
   </si>
   <si>
     <t>1839902295861</t>
-  </si>
-  <si>
-    <t>w</t>
   </si>
   <si>
     <t>1839902267328</t>
@@ -22136,8 +22133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE0E1366-D40A-4A17-B84D-3F0CAAAAF493}">
   <dimension ref="A1:V356"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="22.2" x14ac:dyDescent="0.6"/>
@@ -22385,7 +22382,7 @@
         <v>12</v>
       </c>
       <c r="J4" s="20" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
       <c r="K4" s="21" t="s">
         <v>805</v>
@@ -22781,7 +22778,7 @@
         <v>12</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="K10" s="19">
         <v>842436098</v>
@@ -23526,8 +23523,8 @@
       <c r="Q21" s="19">
         <v>20</v>
       </c>
-      <c r="R21" s="19" t="s">
-        <v>2073</v>
+      <c r="R21" s="19">
+        <v>20</v>
       </c>
       <c r="S21" s="19">
         <v>20</v>

</xml_diff>